<commit_message>
character categories appear to be working fine
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary.xlsx
+++ b/make-uniform/production/Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="50">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -140,21 +140,6 @@
     <t>VEH_IN_HH_OTHER</t>
   </si>
   <si>
-    <t>'None'</t>
-  </si>
-  <si>
-    <t>'1'</t>
-  </si>
-  <si>
-    <t>'2'</t>
-  </si>
-  <si>
-    <t>'3'</t>
-  </si>
-  <si>
-    <t>'4 or more'</t>
-  </si>
-  <si>
     <t>four or more</t>
   </si>
   <si>
@@ -183,6 +168,12 @@
   </si>
   <si>
     <t>Operator</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>4 or more</t>
   </si>
 </sst>
 </file>
@@ -603,8 +594,8 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -616,7 +607,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1645,7 +1636,7 @@
         <v>4</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>4</v>
@@ -1659,7 +1650,7 @@
         <v>30</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>31</v>
@@ -1675,8 +1666,8 @@
       <c r="B63" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>39</v>
+      <c r="C63" s="3">
+        <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>31</v>
@@ -1692,8 +1683,8 @@
       <c r="B64" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>40</v>
+      <c r="C64" s="3">
+        <v>2</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>31</v>
@@ -1709,8 +1700,8 @@
       <c r="B65" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>41</v>
+      <c r="C65" s="3">
+        <v>3</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>31</v>
@@ -1727,13 +1718,13 @@
         <v>30</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1741,13 +1732,13 @@
         <v>6</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>32</v>
@@ -1758,13 +1749,13 @@
         <v>6</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C68" s="1">
         <v>2</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>36</v>
@@ -1775,13 +1766,13 @@
         <v>6</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C69" s="1">
         <v>3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>33</v>
@@ -1792,13 +1783,13 @@
         <v>6</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C70" s="1">
         <v>4</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>34</v>
@@ -1809,13 +1800,13 @@
         <v>6</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C71" s="1">
         <v>5</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>35</v>
@@ -1826,16 +1817,16 @@
         <v>6</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C72" s="1">
         <v>6</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1843,16 +1834,16 @@
         <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C73" s="1">
         <v>7</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,13 +1851,13 @@
         <v>6</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>4</v>
@@ -1877,13 +1868,13 @@
         <v>7</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>32</v>
@@ -1894,13 +1885,13 @@
         <v>7</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C76" s="1">
         <v>1</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>36</v>
@@ -1911,13 +1902,13 @@
         <v>7</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C77" s="1">
         <v>2</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>33</v>
@@ -1928,13 +1919,13 @@
         <v>7</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C78" s="1">
         <v>3</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>34</v>
@@ -1945,13 +1936,13 @@
         <v>7</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C79" s="1">
         <v>4</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>35</v>
@@ -1962,16 +1953,16 @@
         <v>7</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C80" s="1">
         <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1979,16 +1970,16 @@
         <v>7</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C81" s="1">
         <v>6</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a few operators
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary.xlsx
+++ b/make-uniform/production/Dictionary.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13545" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Working Dictionary" sheetId="3" r:id="rId1"/>
+    <sheet name="Dictionary" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="68">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -174,6 +174,60 @@
   </si>
   <si>
     <t>4 or more</t>
+  </si>
+  <si>
+    <t>AC Transit</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>eleven</t>
+  </si>
+  <si>
+    <t>twelve</t>
+  </si>
+  <si>
+    <t>thirteen</t>
+  </si>
+  <si>
+    <t>fourteen</t>
+  </si>
+  <si>
+    <t>fifteen</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Q405</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q404</t>
+  </si>
+  <si>
+    <t>Q403</t>
+  </si>
+  <si>
+    <t>County Connection</t>
+  </si>
+  <si>
+    <t>Q227</t>
   </si>
 </sst>
 </file>
@@ -591,11 +645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -658,16 +712,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -675,16 +729,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -695,67 +749,67 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,13 +820,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,13 +837,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -800,13 +854,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -817,13 +871,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -834,13 +888,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,13 +905,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,13 +922,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,13 +939,13 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,7 +956,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -913,70 +967,70 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -987,13 +1041,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,13 +1058,13 @@
         <v>21</v>
       </c>
       <c r="C24" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,13 +1075,13 @@
         <v>21</v>
       </c>
       <c r="C25" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,13 +1092,13 @@
         <v>21</v>
       </c>
       <c r="C26" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,13 +1109,13 @@
         <v>21</v>
       </c>
       <c r="C27" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,13 +1126,13 @@
         <v>21</v>
       </c>
       <c r="C28" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,13 +1143,13 @@
         <v>21</v>
       </c>
       <c r="C29" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,231 +1160,231 @@
         <v>21</v>
       </c>
       <c r="C30" s="1">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C34" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C36" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C37" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C40" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C42" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>17</v>
@@ -1338,206 +1392,206 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C44" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C46" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C49" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C51" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C52" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C53" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C54" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C55" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,16 +1599,16 @@
         <v>6</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C56" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1562,16 +1616,16 @@
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C57" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1579,16 +1633,16 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,50 +1650,50 @@
         <v>6</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C59" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C60" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1647,16 +1701,16 @@
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>48</v>
+        <v>28</v>
+      </c>
+      <c r="C62" s="1">
+        <v>3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1664,16 +1718,16 @@
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C63" s="3">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C63" s="1">
+        <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1681,16 +1735,16 @@
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C64" s="3">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="C64" s="1">
+        <v>5</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,16 +1752,16 @@
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65" s="3">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="C65" s="1">
+        <v>6</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1715,271 +1769,1308 @@
         <v>7</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="C66" s="1">
+        <v>7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C68" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C69" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C70" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C71" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C72" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C73" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C74" s="1">
+        <v>3</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C75" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C76" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C77" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C78" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C79" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C80" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C81" s="1">
+        <v>10</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C82" s="1">
+        <v>11</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" s="1">
+        <v>12</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="1">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C86" s="1">
+        <v>3</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C87" s="1">
+        <v>4</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" s="1">
+        <v>5</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="3">
+        <v>1</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C93" s="3">
+        <v>3</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C97" s="3">
+        <v>3</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C98" s="3">
+        <v>4</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" s="3">
+        <v>5</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="3">
+        <v>6</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C101" s="3">
+        <v>7</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C102" s="3">
+        <v>8</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C103" s="3">
+        <v>9</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C104" s="3">
+        <v>10</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C105" s="3">
+        <v>11</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" s="3">
+        <v>12</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C107" s="3">
+        <v>13</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C108" s="3">
+        <v>14</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C109" s="3">
+        <v>15</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C110" s="3">
+        <v>16</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C111" s="3">
+        <v>17</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C113" s="1">
+        <v>2</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C114" s="1">
+        <v>3</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C115" s="1">
+        <v>4</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C116" s="1">
+        <v>5</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C117" s="1">
+        <v>6</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C118" s="1">
+        <v>7</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C81" s="1">
-        <v>6</v>
-      </c>
-      <c r="D81" s="1" t="s">
+      <c r="C120" s="1">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E120" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C122" s="1">
+        <v>2</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C123" s="1">
+        <v>3</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C124" s="1">
+        <v>4</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C125" s="1">
+        <v>5</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C126" s="1">
+        <v>6</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E126" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C127" s="1">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C128" s="1">
+        <v>2</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C129" s="1">
+        <v>3</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C130" s="1">
+        <v>4</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C131" s="1">
+        <v>5</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C132" s="1">
+        <v>6</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C133" s="1">
+        <v>7</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C134" s="1">
+        <v>8</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C135" s="1">
+        <v>9</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C136" s="1">
+        <v>10</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C137" s="1">
+        <v>11</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C138" s="1">
+        <v>12</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C139" s="1">
+        <v>13</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C140" s="1">
+        <v>14</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C141" s="1">
+        <v>15</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C142" s="1">
+        <v>16</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ggt added; cccta finished
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary.xlsx
+++ b/make-uniform/production/Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="74">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>Q227</t>
+  </si>
+  <si>
+    <t>Q226</t>
+  </si>
+  <si>
+    <t>Q225</t>
+  </si>
+  <si>
+    <t>Golden Gate Transit</t>
+  </si>
+  <si>
+    <t>Q408</t>
+  </si>
+  <si>
+    <t>Q407</t>
+  </si>
+  <si>
+    <t>Q406</t>
   </si>
 </sst>
 </file>
@@ -645,11 +663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -746,16 +764,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -763,16 +781,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
@@ -780,16 +798,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>4</v>
@@ -797,10 +815,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -814,36 +832,36 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2</v>
+        <v>71</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,13 +872,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -871,13 +889,13 @@
         <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -888,13 +906,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -905,13 +923,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,13 +940,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,13 +957,13 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -956,13 +974,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,13 +991,13 @@
         <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,13 +1008,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1007,13 +1025,13 @@
         <v>9</v>
       </c>
       <c r="C21" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,47 +1042,47 @@
         <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,13 +1093,13 @@
         <v>21</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,13 +1110,13 @@
         <v>21</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,13 +1127,13 @@
         <v>21</v>
       </c>
       <c r="C27" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1126,13 +1144,13 @@
         <v>21</v>
       </c>
       <c r="C28" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1143,13 +1161,13 @@
         <v>21</v>
       </c>
       <c r="C29" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,13 +1178,13 @@
         <v>21</v>
       </c>
       <c r="C30" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,13 +1195,13 @@
         <v>21</v>
       </c>
       <c r="C31" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1194,13 +1212,13 @@
         <v>21</v>
       </c>
       <c r="C32" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,13 +1229,13 @@
         <v>21</v>
       </c>
       <c r="C33" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1228,47 +1246,47 @@
         <v>21</v>
       </c>
       <c r="C34" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C35" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C36" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,13 +1297,13 @@
         <v>62</v>
       </c>
       <c r="C37" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,13 +1314,13 @@
         <v>62</v>
       </c>
       <c r="C38" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,13 +1331,13 @@
         <v>62</v>
       </c>
       <c r="C39" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,13 +1348,13 @@
         <v>62</v>
       </c>
       <c r="C40" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,13 +1365,13 @@
         <v>62</v>
       </c>
       <c r="C41" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,13 +1382,13 @@
         <v>62</v>
       </c>
       <c r="C42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,13 +1399,13 @@
         <v>62</v>
       </c>
       <c r="C43" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,13 +1416,13 @@
         <v>62</v>
       </c>
       <c r="C44" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,13 +1433,13 @@
         <v>62</v>
       </c>
       <c r="C45" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,265 +1450,265 @@
         <v>62</v>
       </c>
       <c r="C46" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C47" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C48" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C49" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C50" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C51" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C52" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C54" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C55" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C56" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C57" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C59" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C60" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C61" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>11</v>
@@ -1698,16 +1716,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C62" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>12</v>
@@ -1715,50 +1733,50 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C63" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C64" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C65" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>14</v>
@@ -1766,67 +1784,67 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C67" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C68" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C69" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>17</v>
@@ -1834,33 +1852,33 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C70" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C71" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>18</v>
@@ -1868,149 +1886,149 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C72" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C73" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C74" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C75" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C76" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C77" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C79" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C80" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>27</v>
@@ -2021,30 +2039,30 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C81" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C82" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>27</v>
@@ -2055,19 +2073,19 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C83" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2075,16 +2093,16 @@
         <v>6</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C84" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2092,84 +2110,84 @@
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C85" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C86" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C87" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C88" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C89" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C89" s="1">
         <v>4</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2177,16 +2195,16 @@
         <v>7</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>48</v>
+        <v>28</v>
+      </c>
+      <c r="C90" s="1">
+        <v>5</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2194,16 +2212,16 @@
         <v>7</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C91" s="3">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C91" s="1">
+        <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2211,16 +2229,16 @@
         <v>7</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C92" s="3">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="C92" s="1">
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2228,16 +2246,16 @@
         <v>7</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C93" s="3">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="C93" s="1">
+        <v>8</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2245,67 +2263,67 @@
         <v>7</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="C94" s="1">
+        <v>10</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C95" s="3">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C95" s="1">
+        <v>11</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C96" s="3">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="C96" s="1">
+        <v>13</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C97" s="3">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="C97" s="1">
+        <v>15</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2313,16 +2331,16 @@
         <v>50</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C98" s="3">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2330,16 +2348,16 @@
         <v>50</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C99" s="3">
-        <v>5</v>
+        <v>63</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,16 +2365,16 @@
         <v>50</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" s="3">
-        <v>6</v>
+        <v>63</v>
+      </c>
+      <c r="C100" s="1">
+        <v>3</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2364,16 +2382,16 @@
         <v>50</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C101" s="3">
-        <v>7</v>
+        <v>63</v>
+      </c>
+      <c r="C101" s="1">
+        <v>4</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2381,16 +2399,16 @@
         <v>50</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C102" s="3">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="C102" s="1">
+        <v>5</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,16 +2416,16 @@
         <v>50</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C103" s="3">
-        <v>9</v>
+        <v>63</v>
+      </c>
+      <c r="C103" s="1">
+        <v>6</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2415,16 +2433,16 @@
         <v>50</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C104" s="3">
-        <v>10</v>
+        <v>63</v>
+      </c>
+      <c r="C104" s="1">
+        <v>7</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2432,16 +2450,16 @@
         <v>50</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C105" s="3">
-        <v>11</v>
+        <v>63</v>
+      </c>
+      <c r="C105" s="1">
+        <v>8</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2449,16 +2467,16 @@
         <v>50</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C106" s="3">
-        <v>12</v>
+        <v>63</v>
+      </c>
+      <c r="C106" s="1">
+        <v>9</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2466,16 +2484,16 @@
         <v>50</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C107" s="3">
-        <v>13</v>
+        <v>63</v>
+      </c>
+      <c r="C107" s="1">
+        <v>10</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2483,16 +2501,16 @@
         <v>50</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C108" s="3">
-        <v>14</v>
+        <v>63</v>
+      </c>
+      <c r="C108" s="1">
+        <v>11</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,577 +2518,2583 @@
         <v>50</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C109" s="3">
-        <v>15</v>
+        <v>63</v>
+      </c>
+      <c r="C109" s="1">
+        <v>12</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C110" s="3">
-        <v>16</v>
+        <v>63</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C111" s="3">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="C111" s="1">
+        <v>2</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C112" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C113" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C114" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C115" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C116" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C117" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C118" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
+      </c>
+      <c r="C119" s="1">
+        <v>10</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C120" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C121" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C122" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C123" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C124" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C125" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C126" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C127" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C128" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C129" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C130" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C131" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C132" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C133" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C134" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C135" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C136" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C137" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C138" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C139" s="1">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C140" s="1">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C141" s="1">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="C141" s="3">
+        <v>1</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C143" s="3">
+        <v>3</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C145" s="3">
+        <v>1</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C147" s="3">
+        <v>3</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C148" s="3">
+        <v>4</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C149" s="3">
+        <v>5</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C150" s="3">
+        <v>6</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C151" s="3">
+        <v>7</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C152" s="3">
+        <v>8</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C153" s="3">
+        <v>9</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C154" s="3">
+        <v>10</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C155" s="3">
+        <v>11</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C156" s="3">
+        <v>12</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C157" s="3">
+        <v>13</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C158" s="3">
+        <v>14</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C159" s="3">
+        <v>15</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C160" s="3">
+        <v>16</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C161" s="3">
+        <v>17</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C162" s="3">
+        <v>1</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C163" s="3">
+        <v>2</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C164" s="3">
+        <v>3</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C165" s="3">
+        <v>4</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C166" s="3">
+        <v>5</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C167" s="3">
+        <v>6</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C168" s="3">
+        <v>7</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C169" s="3">
+        <v>8</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C170" s="3">
+        <v>9</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C171" s="3">
+        <v>10</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C172" s="3">
+        <v>11</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C173" s="3">
+        <v>12</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C174" s="3">
+        <v>13</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C175" s="3">
+        <v>14</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C176" s="3">
+        <v>15</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C177" s="3">
+        <v>16</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C178" s="3">
+        <v>17</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C179" s="3">
+        <v>1</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C180" s="3">
+        <v>2</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C181" s="3">
+        <v>3</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C182" s="3">
+        <v>4</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C183" s="3">
+        <v>5</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C184" s="3">
+        <v>6</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C185" s="3">
+        <v>7</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C186" s="3">
+        <v>8</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C187" s="3">
+        <v>9</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C188" s="3">
+        <v>10</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C189" s="3">
+        <v>11</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C190" s="3">
+        <v>12</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C191" s="3">
+        <v>13</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C192" s="3">
+        <v>14</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C193" s="3">
+        <v>15</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C194" s="3">
+        <v>16</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C195" s="3">
+        <v>17</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C196" s="1">
+        <v>1</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C197" s="1">
+        <v>2</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C198" s="1">
+        <v>3</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C199" s="1">
+        <v>4</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C200" s="1">
+        <v>5</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C201" s="1">
+        <v>6</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C202" s="1">
+        <v>7</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C204" s="1">
+        <v>0</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C205" s="1">
+        <v>1</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C206" s="1">
+        <v>2</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C207" s="1">
+        <v>3</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C208" s="1">
+        <v>4</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C209" s="1">
+        <v>5</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C210" s="1">
+        <v>6</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C211" s="1">
+        <v>1</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C212" s="1">
+        <v>2</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C213" s="1">
+        <v>3</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C214" s="1">
+        <v>4</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C215" s="1">
+        <v>5</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C216" s="1">
+        <v>6</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C217" s="1">
+        <v>7</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C218" s="1">
+        <v>8</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C219" s="1">
+        <v>9</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C220" s="1">
+        <v>10</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C221" s="1">
+        <v>11</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C222" s="1">
+        <v>12</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C223" s="1">
+        <v>13</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C224" s="1">
+        <v>14</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C225" s="1">
+        <v>15</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C226" s="1">
         <v>16</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E142" s="1" t="s">
+      <c r="D226" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E226" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C227" s="1">
+        <v>1</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C228" s="1">
+        <v>2</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C229" s="1">
+        <v>3</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C230" s="1">
+        <v>4</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C231" s="1">
+        <v>5</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C232" s="1">
+        <v>6</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C233" s="1">
+        <v>7</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C234" s="1">
+        <v>8</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C235" s="1">
+        <v>9</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C236" s="1">
+        <v>10</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C237" s="1">
+        <v>11</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C238" s="1">
+        <v>12</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C239" s="1">
+        <v>13</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C240" s="1">
+        <v>14</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C241" s="1">
+        <v>15</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C242" s="1">
+        <v>16</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C243" s="1">
+        <v>17</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C244" s="1">
+        <v>1</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C245" s="1">
+        <v>2</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C246" s="1">
+        <v>3</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C247" s="1">
+        <v>4</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C248" s="1">
+        <v>5</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C249" s="1">
+        <v>6</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C250" s="1">
+        <v>7</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C251" s="1">
+        <v>8</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C252" s="1">
+        <v>9</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C253" s="1">
+        <v>10</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C254" s="1">
+        <v>11</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C255" s="1">
+        <v>12</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C256" s="1">
+        <v>13</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C257" s="1">
+        <v>14</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C258" s="1">
+        <v>15</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C259" s="1">
+        <v>16</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C260" s="1">
+        <v>17</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added garbage collection, progress on caltrain
steady as she goes
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary.xlsx
+++ b/make-uniform/production/Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="161">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -387,6 +387,126 @@
   </si>
   <si>
     <t>WILL_GO2SCHOOL_TODAY</t>
+  </si>
+  <si>
+    <t>HOME_LAT</t>
+  </si>
+  <si>
+    <t>HOME_LON</t>
+  </si>
+  <si>
+    <t>WORKP_LAT</t>
+  </si>
+  <si>
+    <t>workplace_lat</t>
+  </si>
+  <si>
+    <t>home_lat</t>
+  </si>
+  <si>
+    <t>home_lon</t>
+  </si>
+  <si>
+    <t>WORKP_LON</t>
+  </si>
+  <si>
+    <t>workplace_lon</t>
+  </si>
+  <si>
+    <t>SCHOOL_LAT</t>
+  </si>
+  <si>
+    <t>school_lat</t>
+  </si>
+  <si>
+    <t>SCHOOL_LON</t>
+  </si>
+  <si>
+    <t>school_lon</t>
+  </si>
+  <si>
+    <t>DESTINATION_LAT</t>
+  </si>
+  <si>
+    <t>dest_lat</t>
+  </si>
+  <si>
+    <t>DESTINATION_LON</t>
+  </si>
+  <si>
+    <t>dest_lon</t>
+  </si>
+  <si>
+    <t>ORIGIN_LAT</t>
+  </si>
+  <si>
+    <t>orig_lat</t>
+  </si>
+  <si>
+    <t>ORIGIN_LON</t>
+  </si>
+  <si>
+    <t>orig_lon</t>
+  </si>
+  <si>
+    <t>ENTER_STATION_LAT</t>
+  </si>
+  <si>
+    <t>survey_board_lat</t>
+  </si>
+  <si>
+    <t>survey_board_lon</t>
+  </si>
+  <si>
+    <t>ENTER_STATION_LON</t>
+  </si>
+  <si>
+    <t>ENTER_STATION</t>
+  </si>
+  <si>
+    <t>survey_board_name</t>
+  </si>
+  <si>
+    <t>EXIT_STATION_LAT</t>
+  </si>
+  <si>
+    <t>EXIT_STATION_LON</t>
+  </si>
+  <si>
+    <t>EXIT_STATION</t>
+  </si>
+  <si>
+    <t>survey_alight_lat</t>
+  </si>
+  <si>
+    <t>survey_alight_lon</t>
+  </si>
+  <si>
+    <t>survey_alight_name</t>
+  </si>
+  <si>
+    <t>EGRESS_LOC_LAT_TRANSFER_TO_LAST</t>
+  </si>
+  <si>
+    <t>last_alight_lat</t>
+  </si>
+  <si>
+    <t>EGRESS_LOC_LON_TRANSFER_TO_LAST</t>
+  </si>
+  <si>
+    <t>last_alight_lon</t>
+  </si>
+  <si>
+    <t>ACCESS_LOC_LAT_TRANSFER_FROM_1ST</t>
+  </si>
+  <si>
+    <t>first_board_lat</t>
+  </si>
+  <si>
+    <t>ACCESS_LOC_LON_TRANSFER_FROM_1ST</t>
+  </si>
+  <si>
+    <t>first_board_lon</t>
   </si>
 </sst>
 </file>
@@ -804,17 +924,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E525"/>
+  <dimension ref="A1:E545"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A518" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A546" sqref="A546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.625" style="1" customWidth="1"/>
@@ -9743,6 +9863,346 @@
       </c>
       <c r="E525" s="1" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A526" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C526" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D526" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E526" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A527" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C527" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D527" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E527" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A528" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C528" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D528" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E528" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A529" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C529" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D529" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E529" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A530" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C530" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D530" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E530" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A531" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D531" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E531" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A532" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E532" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A533" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D533" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E533" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A534" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C534" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D534" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E534" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A535" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C535" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D535" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E535" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A536" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C536" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D536" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E536" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A537" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C537" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D537" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E537" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A538" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C538" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D538" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E538" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A539" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C539" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D539" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E539" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A540" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C540" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D540" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E540" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A541" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C541" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D541" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E541" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A542" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D542" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E542" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A543" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B543" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C543" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D543" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E543" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A544" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D544" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E544" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A545" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C545" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D545" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E545" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small steps on transfer sequence
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary.xlsx
+++ b/make-uniform/production/Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="182">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -507,6 +507,69 @@
   </si>
   <si>
     <t>first_board_lon</t>
+  </si>
+  <si>
+    <t>onoff_enter_station</t>
+  </si>
+  <si>
+    <t>onoff_exit_station</t>
+  </si>
+  <si>
+    <t>TRANSFERS_FROM_CODE</t>
+  </si>
+  <si>
+    <t>3+</t>
+  </si>
+  <si>
+    <t>origin_survey_board_transfers</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>three or more</t>
+  </si>
+  <si>
+    <t>TRANSFERS_TO_CODE</t>
+  </si>
+  <si>
+    <t>TRANSFER_FROM_1ST</t>
+  </si>
+  <si>
+    <t>first_route_before_survey_board</t>
+  </si>
+  <si>
+    <t>TRANSFER_FROM_2ND</t>
+  </si>
+  <si>
+    <t>second_route_before_survey_board</t>
+  </si>
+  <si>
+    <t>TRANSFER_FROM_3RD</t>
+  </si>
+  <si>
+    <t>third_route_before_survey_board</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_1ST</t>
+  </si>
+  <si>
+    <t>first_route_after_survey_alight</t>
+  </si>
+  <si>
+    <t>survey_alight_dest_transfers</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_2ND</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_3RD</t>
+  </si>
+  <si>
+    <t>second_route_after_survey_alight</t>
+  </si>
+  <si>
+    <t>third_route_after_survey_alight</t>
   </si>
 </sst>
 </file>
@@ -924,11 +987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E545"/>
+  <dimension ref="A1:E561"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A518" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A546" sqref="A546"/>
+      <pane ySplit="1" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A562" sqref="A562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -936,7 +999,7 @@
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10202,6 +10265,278 @@
         <v>160</v>
       </c>
       <c r="E545" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A546" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B546" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C546" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D546" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E546" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A547" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C547" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D547" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E547" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A548" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C548" s="1">
+        <v>0</v>
+      </c>
+      <c r="D548" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E548" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A549" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C549" s="1">
+        <v>1</v>
+      </c>
+      <c r="D549" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E549" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A550" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C550" s="1">
+        <v>2</v>
+      </c>
+      <c r="D550" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E550" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A551" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C551" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D551" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E551" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A552" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C552" s="1">
+        <v>0</v>
+      </c>
+      <c r="D552" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E552" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A553" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C553" s="1">
+        <v>1</v>
+      </c>
+      <c r="D553" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E553" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A554" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C554" s="1">
+        <v>2</v>
+      </c>
+      <c r="D554" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E554" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A555" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C555" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D555" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E555" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A556" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C556" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D556" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E556" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A557" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C557" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D557" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E557" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A558" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C558" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D558" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E558" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A559" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C559" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D559" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E559" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A560" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E560" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A561" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C561" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D561" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E561" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
progress on tech, oper, paths
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary.xlsx
+++ b/make-uniform/production/Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="190">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -570,6 +570,30 @@
   </si>
   <si>
     <t>third_route_after_survey_alight</t>
+  </si>
+  <si>
+    <t>ACCESS_MODE_CODE</t>
+  </si>
+  <si>
+    <t>access_mode</t>
+  </si>
+  <si>
+    <t>walk</t>
+  </si>
+  <si>
+    <t>bike</t>
+  </si>
+  <si>
+    <t>pnr</t>
+  </si>
+  <si>
+    <t>knr</t>
+  </si>
+  <si>
+    <t>EGRESS_MODE_CODE</t>
+  </si>
+  <si>
+    <t>egress_mode</t>
   </si>
 </sst>
 </file>
@@ -987,11 +1011,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E561"/>
+  <dimension ref="A1:E579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A562" sqref="A562"/>
+      <pane ySplit="1" topLeftCell="A548" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A580" sqref="A580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10540,6 +10564,312 @@
         <v>4</v>
       </c>
     </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A562" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C562" s="1">
+        <v>1</v>
+      </c>
+      <c r="D562" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E562" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A563" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C563" s="1">
+        <v>2</v>
+      </c>
+      <c r="D563" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E563" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A564" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C564" s="1">
+        <v>3</v>
+      </c>
+      <c r="D564" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E564" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A565" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C565" s="1">
+        <v>4</v>
+      </c>
+      <c r="D565" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E565" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A566" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C566" s="1">
+        <v>5</v>
+      </c>
+      <c r="D566" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E566" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A567" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C567" s="1">
+        <v>6</v>
+      </c>
+      <c r="D567" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E567" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A568" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C568" s="1">
+        <v>7</v>
+      </c>
+      <c r="D568" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E568" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A569" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C569" s="1">
+        <v>8</v>
+      </c>
+      <c r="D569" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E569" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A570" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C570" s="1">
+        <v>9</v>
+      </c>
+      <c r="D570" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E570" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A571" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C571" s="1">
+        <v>1</v>
+      </c>
+      <c r="D571" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E571" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A572" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C572" s="1">
+        <v>2</v>
+      </c>
+      <c r="D572" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E572" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A573" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C573" s="1">
+        <v>3</v>
+      </c>
+      <c r="D573" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E573" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A574" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C574" s="1">
+        <v>4</v>
+      </c>
+      <c r="D574" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E574" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A575" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C575" s="1">
+        <v>5</v>
+      </c>
+      <c r="D575" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E575" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A576" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C576" s="1">
+        <v>6</v>
+      </c>
+      <c r="D576" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E576" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A577" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C577" s="1">
+        <v>7</v>
+      </c>
+      <c r="D577" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E577" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A578" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C578" s="1">
+        <v>8</v>
+      </c>
+      <c r="D578" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E578" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="579" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A579" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C579" s="1">
+        <v>9</v>
+      </c>
+      <c r="D579" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E579" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>